<commit_message>
updated Atrybuty.xlsx, Encje.xlsx, Relacje.xlsx
</commit_message>
<xml_diff>
--- a/work/r5/Atrybuty.xlsx
+++ b/work/r5/Atrybuty.xlsx
@@ -43,25 +43,7 @@
     <t xml:space="preserve">Tak</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Customer</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">FirstName</t>
-    </r>
+    <t xml:space="preserve">CustomerFirstName</t>
   </si>
   <si>
     <t xml:space="preserve">Ciąg znaków</t>
@@ -70,139 +52,31 @@
     <t xml:space="preserve">Nie</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Customer</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">LastName</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Customer</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Email</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Customer</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">PhoneNumber</t>
-    </r>
+    <t xml:space="preserve">CustomerLastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CustomerEmail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CustomerPhoneNumber</t>
   </si>
   <si>
     <t xml:space="preserve">CustomerAddress</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Customer</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Birthday</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">?DATE</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Customer</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Password</t>
-    </r>
+    <t xml:space="preserve">CustomerBirthday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CustomerPassword</t>
   </si>
   <si>
     <t xml:space="preserve">CustomerCreationDate</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Customer</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ModificationDate</t>
-    </r>
+    <t xml:space="preserve">CustomerModificationDate</t>
   </si>
   <si>
     <t xml:space="preserve">CityKey</t>
@@ -401,6 +275,7 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -412,6 +287,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -435,7 +311,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -444,31 +320,17 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="thick"/>
-      <right style="thick"/>
-      <top style="thick"/>
-      <bottom style="thick"/>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium"/>
-      <top/>
-      <bottom style="medium"/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -497,7 +359,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -507,14 +369,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -522,20 +376,16 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -555,21 +405,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="19.09"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.61"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -583,7 +433,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -597,8 +447,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+    <row r="3" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -611,8 +461,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+    <row r="4" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -625,8 +475,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+    <row r="5" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -639,8 +489,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+    <row r="6" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -653,8 +503,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+    <row r="7" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -667,8 +517,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+    <row r="8" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -681,8 +531,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+    <row r="9" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -695,8 +545,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+    <row r="10" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -709,8 +559,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
+    <row r="11" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -723,7 +573,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
@@ -737,7 +587,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
         <v>20</v>
       </c>
@@ -751,7 +601,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
         <v>21</v>
       </c>
@@ -765,7 +615,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
@@ -778,8 +628,9 @@
       <c r="D15" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
@@ -793,7 +644,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
         <v>24</v>
       </c>
@@ -807,7 +658,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
@@ -821,7 +672,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
         <v>26</v>
       </c>
@@ -835,7 +686,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
         <v>27</v>
       </c>
@@ -849,7 +700,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
         <v>28</v>
       </c>
@@ -863,7 +714,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
         <v>29</v>
       </c>
@@ -877,7 +728,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
         <v>30</v>
       </c>
@@ -891,7 +742,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
         <v>31</v>
       </c>
@@ -905,7 +756,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
         <v>32</v>
       </c>
@@ -919,7 +770,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
         <v>33</v>
       </c>
@@ -933,7 +784,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
         <v>35</v>
       </c>
@@ -947,7 +798,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
         <v>36</v>
       </c>
@@ -961,7 +812,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
         <v>37</v>
       </c>
@@ -975,7 +826,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
         <v>38</v>
       </c>
@@ -989,7 +840,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
@@ -1003,7 +854,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
         <v>40</v>
       </c>
@@ -1017,7 +868,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
         <v>41</v>
       </c>
@@ -1031,7 +882,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
         <v>43</v>
       </c>
@@ -1045,7 +896,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
         <v>44</v>
       </c>
@@ -1059,7 +910,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
         <v>45</v>
       </c>
@@ -1073,7 +924,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
         <v>46</v>
       </c>
@@ -1087,7 +938,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
         <v>47</v>
       </c>
@@ -1101,7 +952,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
         <v>48</v>
       </c>
@@ -1115,7 +966,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
         <v>49</v>
       </c>
@@ -1129,7 +980,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
         <v>50</v>
       </c>
@@ -1143,7 +994,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
         <v>51</v>
       </c>
@@ -1157,7 +1008,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
         <v>52</v>
       </c>
@@ -1171,7 +1022,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
         <v>53</v>
       </c>
@@ -1185,7 +1036,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
         <v>54</v>
       </c>
@@ -1199,7 +1050,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
         <v>55</v>
       </c>
@@ -1213,7 +1064,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
         <v>56</v>
       </c>
@@ -1227,7 +1078,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
         <v>57</v>
       </c>
@@ -1241,7 +1092,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
         <v>58</v>
       </c>
@@ -1255,7 +1106,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
         <v>59</v>
       </c>
@@ -1269,7 +1120,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
         <v>60</v>
       </c>
@@ -1283,7 +1134,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
         <v>61</v>
       </c>
@@ -1297,7 +1148,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
         <v>62</v>
       </c>
@@ -1311,7 +1162,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
         <v>63</v>
       </c>
@@ -1325,7 +1176,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
         <v>64</v>
       </c>
@@ -1339,7 +1190,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
         <v>65</v>
       </c>
@@ -1353,7 +1204,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
         <v>66</v>
       </c>
@@ -1367,7 +1218,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="6" t="s">
         <v>67</v>
       </c>
@@ -1381,8 +1232,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="7" t="s">
+    <row r="59" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B59" s="4" t="s">
@@ -1395,8 +1246,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="7" t="s">
+    <row r="60" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B60" s="4" t="s">
@@ -1409,8 +1260,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="7" t="s">
+    <row r="61" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="3" t="s">
         <v>70</v>
       </c>
       <c r="B61" s="4" t="s">
@@ -1423,8 +1274,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="7" t="s">
+    <row r="62" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B62" s="4" t="s">
@@ -1437,8 +1288,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="7" t="s">
+    <row r="63" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="3" t="s">
         <v>72</v>
       </c>
       <c r="B63" s="4" t="s">
@@ -1451,8 +1302,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="7" t="s">
+    <row r="64" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="3" t="s">
         <v>73</v>
       </c>
       <c r="B64" s="4" t="s">
@@ -1465,17 +1316,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="8" t="s">
+    <row r="65" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B65" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D65" s="9" t="s">
+      <c r="B65" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" s="4" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Merge rozdzial5, rozdzial6 into main-merge:   v2
</commit_message>
<xml_diff>
--- a/work/r5/Atrybuty.xlsx
+++ b/work/r5/Atrybuty.xlsx
@@ -43,25 +43,7 @@
     <t xml:space="preserve">Tak</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Customer</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">FirstName</t>
-    </r>
+    <t xml:space="preserve">CustomerFirstName</t>
   </si>
   <si>
     <t xml:space="preserve">Ciąg znaków</t>
@@ -70,139 +52,31 @@
     <t xml:space="preserve">Nie</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Customer</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">LastName</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Customer</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Email</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Customer</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">PhoneNumber</t>
-    </r>
+    <t xml:space="preserve">CustomerLastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CustomerEmail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CustomerPhoneNumber</t>
   </si>
   <si>
     <t xml:space="preserve">CustomerAddress</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Customer</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Birthday</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">?DATE</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Customer</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Password</t>
-    </r>
+    <t xml:space="preserve">CustomerBirthday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CustomerPassword</t>
   </si>
   <si>
     <t xml:space="preserve">CustomerCreationDate</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Customer</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ModificationDate</t>
-    </r>
+    <t xml:space="preserve">CustomerModificationDate</t>
   </si>
   <si>
     <t xml:space="preserve">CityKey</t>
@@ -401,6 +275,7 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -412,6 +287,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -435,7 +311,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -444,31 +320,17 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="thick"/>
-      <right style="thick"/>
-      <top style="thick"/>
-      <bottom style="thick"/>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium"/>
-      <top/>
-      <bottom style="medium"/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -497,7 +359,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -507,14 +369,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -522,20 +376,16 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -555,21 +405,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="19.09"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.61"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -583,7 +433,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -597,8 +447,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+    <row r="3" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -611,8 +461,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+    <row r="4" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -625,8 +475,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+    <row r="5" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -639,8 +489,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+    <row r="6" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -653,8 +503,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+    <row r="7" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -667,8 +517,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+    <row r="8" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -681,8 +531,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+    <row r="9" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -695,8 +545,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+    <row r="10" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -709,8 +559,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
+    <row r="11" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -723,7 +573,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
@@ -737,7 +587,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
         <v>20</v>
       </c>
@@ -751,7 +601,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
         <v>21</v>
       </c>
@@ -765,7 +615,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
@@ -778,8 +628,9 @@
       <c r="D15" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
@@ -793,7 +644,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
         <v>24</v>
       </c>
@@ -807,7 +658,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
@@ -821,7 +672,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
         <v>26</v>
       </c>
@@ -835,7 +686,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
         <v>27</v>
       </c>
@@ -849,7 +700,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
         <v>28</v>
       </c>
@@ -863,7 +714,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
         <v>29</v>
       </c>
@@ -877,7 +728,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
         <v>30</v>
       </c>
@@ -891,7 +742,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
         <v>31</v>
       </c>
@@ -905,7 +756,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
         <v>32</v>
       </c>
@@ -919,7 +770,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
         <v>33</v>
       </c>
@@ -933,7 +784,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
         <v>35</v>
       </c>
@@ -947,7 +798,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
         <v>36</v>
       </c>
@@ -961,7 +812,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
         <v>37</v>
       </c>
@@ -975,7 +826,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
         <v>38</v>
       </c>
@@ -989,7 +840,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
@@ -1003,7 +854,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
         <v>40</v>
       </c>
@@ -1017,7 +868,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
         <v>41</v>
       </c>
@@ -1031,7 +882,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
         <v>43</v>
       </c>
@@ -1045,7 +896,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
         <v>44</v>
       </c>
@@ -1059,7 +910,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
         <v>45</v>
       </c>
@@ -1073,7 +924,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
         <v>46</v>
       </c>
@@ -1087,7 +938,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
         <v>47</v>
       </c>
@@ -1101,7 +952,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
         <v>48</v>
       </c>
@@ -1115,7 +966,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
         <v>49</v>
       </c>
@@ -1129,7 +980,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
         <v>50</v>
       </c>
@@ -1143,7 +994,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
         <v>51</v>
       </c>
@@ -1157,7 +1008,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
         <v>52</v>
       </c>
@@ -1171,7 +1022,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
         <v>53</v>
       </c>
@@ -1185,7 +1036,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
         <v>54</v>
       </c>
@@ -1199,7 +1050,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
         <v>55</v>
       </c>
@@ -1213,7 +1064,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
         <v>56</v>
       </c>
@@ -1227,7 +1078,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
         <v>57</v>
       </c>
@@ -1241,7 +1092,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
         <v>58</v>
       </c>
@@ -1255,7 +1106,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
         <v>59</v>
       </c>
@@ -1269,7 +1120,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
         <v>60</v>
       </c>
@@ -1283,7 +1134,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
         <v>61</v>
       </c>
@@ -1297,7 +1148,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
         <v>62</v>
       </c>
@@ -1311,7 +1162,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
         <v>63</v>
       </c>
@@ -1325,7 +1176,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
         <v>64</v>
       </c>
@@ -1339,7 +1190,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
         <v>65</v>
       </c>
@@ -1353,7 +1204,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
         <v>66</v>
       </c>
@@ -1367,7 +1218,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="6" t="s">
         <v>67</v>
       </c>
@@ -1381,8 +1232,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="7" t="s">
+    <row r="59" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B59" s="4" t="s">
@@ -1395,8 +1246,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="7" t="s">
+    <row r="60" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B60" s="4" t="s">
@@ -1409,8 +1260,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="7" t="s">
+    <row r="61" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="3" t="s">
         <v>70</v>
       </c>
       <c r="B61" s="4" t="s">
@@ -1423,8 +1274,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="7" t="s">
+    <row r="62" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B62" s="4" t="s">
@@ -1437,8 +1288,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="7" t="s">
+    <row r="63" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="3" t="s">
         <v>72</v>
       </c>
       <c r="B63" s="4" t="s">
@@ -1451,8 +1302,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="7" t="s">
+    <row r="64" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="3" t="s">
         <v>73</v>
       </c>
       <c r="B64" s="4" t="s">
@@ -1465,17 +1316,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="8" t="s">
+    <row r="65" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B65" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D65" s="9" t="s">
+      <c r="B65" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" s="4" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>